<commit_message>
guardar juego de ruleta
</commit_message>
<xml_diff>
--- a/Data/Reporte_juego.xlsx
+++ b/Data/Reporte_juego.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y27"/>
+  <dimension ref="A1:Y29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2308,6 +2308,140 @@
         <v>29</v>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2024-10-10 21:29:36</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="n">
+        <v>33</v>
+      </c>
+      <c r="D28" t="n">
+        <v>10</v>
+      </c>
+      <c r="E28" t="n">
+        <v>23</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="n">
+        <v>10</v>
+      </c>
+      <c r="O28" t="n">
+        <v>10</v>
+      </c>
+      <c r="P28" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q28" t="inlineStr"/>
+      <c r="R28" t="n">
+        <v>5</v>
+      </c>
+      <c r="S28" t="inlineStr"/>
+      <c r="T28" t="n">
+        <v>20</v>
+      </c>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>34%</t>
+        </is>
+      </c>
+      <c r="V28" t="inlineStr">
+        <is>
+          <t>C:\Users\jonat\OneDrive\Escritorio\Repositorio\jonatha1992\Predictor_App\Data\Crupier.xlsx</t>
+        </is>
+      </c>
+      <c r="W28" t="inlineStr"/>
+      <c r="X28" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y28" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2024-10-10 21:58:24</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="n">
+        <v>16</v>
+      </c>
+      <c r="D29" t="n">
+        <v>2</v>
+      </c>
+      <c r="E29" t="n">
+        <v>9</v>
+      </c>
+      <c r="F29" t="n">
+        <v>5</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
+      <c r="N29" t="n">
+        <v>10</v>
+      </c>
+      <c r="O29" t="n">
+        <v>10</v>
+      </c>
+      <c r="P29" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q29" t="inlineStr"/>
+      <c r="R29" t="n">
+        <v>5</v>
+      </c>
+      <c r="S29" t="inlineStr"/>
+      <c r="T29" t="n">
+        <v>20</v>
+      </c>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>47%</t>
+        </is>
+      </c>
+      <c r="V29" t="inlineStr">
+        <is>
+          <t>C:\Users\jonat\OneDrive\Escritorio\Repositorio\jonatha1992\Predictor_App\Data\Crupier.xlsx</t>
+        </is>
+      </c>
+      <c r="W29" t="inlineStr"/>
+      <c r="X29" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y29" t="n">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
5500 tiradas de juego electromecanica
</commit_message>
<xml_diff>
--- a/Data/Reporte_juego.xlsx
+++ b/Data/Reporte_juego.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y40"/>
+  <dimension ref="A1:Y41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3179,6 +3179,73 @@
         <v>0</v>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2024-10-14 22:02:12</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr"/>
+      <c r="C41" t="n">
+        <v>10</v>
+      </c>
+      <c r="D41" t="n">
+        <v>3</v>
+      </c>
+      <c r="E41" t="n">
+        <v>7</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="inlineStr"/>
+      <c r="K41" t="inlineStr"/>
+      <c r="L41" t="inlineStr"/>
+      <c r="M41" t="inlineStr"/>
+      <c r="N41" t="n">
+        <v>10</v>
+      </c>
+      <c r="O41" t="n">
+        <v>10</v>
+      </c>
+      <c r="P41" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q41" t="inlineStr"/>
+      <c r="R41" t="n">
+        <v>5</v>
+      </c>
+      <c r="S41" t="inlineStr"/>
+      <c r="T41" t="n">
+        <v>20</v>
+      </c>
+      <c r="U41" t="inlineStr">
+        <is>
+          <t>25%</t>
+        </is>
+      </c>
+      <c r="V41" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W41" t="inlineStr"/>
+      <c r="X41" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y41" t="n">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
eliminacion de buqueda de parametros y jugadas en electromecanica
</commit_message>
<xml_diff>
--- a/Data/Reporte_juego.xlsx
+++ b/Data/Reporte_juego.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y40"/>
+  <dimension ref="A1:Y43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3179,6 +3179,207 @@
         <v>0</v>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2024-10-16 22:53:42</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr"/>
+      <c r="C41" t="n">
+        <v>13</v>
+      </c>
+      <c r="D41" t="n">
+        <v>4</v>
+      </c>
+      <c r="E41" t="n">
+        <v>9</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="inlineStr"/>
+      <c r="K41" t="inlineStr"/>
+      <c r="L41" t="inlineStr"/>
+      <c r="M41" t="inlineStr"/>
+      <c r="N41" t="n">
+        <v>10</v>
+      </c>
+      <c r="O41" t="n">
+        <v>10</v>
+      </c>
+      <c r="P41" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q41" t="inlineStr"/>
+      <c r="R41" t="n">
+        <v>5</v>
+      </c>
+      <c r="S41" t="inlineStr"/>
+      <c r="T41" t="n">
+        <v>20</v>
+      </c>
+      <c r="U41" t="inlineStr">
+        <is>
+          <t>26%</t>
+        </is>
+      </c>
+      <c r="V41" t="inlineStr">
+        <is>
+          <t>C:\Users\jonat\OneDrive\Escritorio\Repositorio\jonatha1992\Predictor_App\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W41" t="inlineStr"/>
+      <c r="X41" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y41" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2024-10-19 00:27:08</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr"/>
+      <c r="C42" t="n">
+        <v>2</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" t="n">
+        <v>2</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="inlineStr"/>
+      <c r="K42" t="inlineStr"/>
+      <c r="L42" t="inlineStr"/>
+      <c r="M42" t="inlineStr"/>
+      <c r="N42" t="n">
+        <v>10</v>
+      </c>
+      <c r="O42" t="n">
+        <v>10</v>
+      </c>
+      <c r="P42" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q42" t="inlineStr"/>
+      <c r="R42" t="n">
+        <v>5</v>
+      </c>
+      <c r="S42" t="inlineStr"/>
+      <c r="T42" t="n">
+        <v>20</v>
+      </c>
+      <c r="U42" t="inlineStr">
+        <is>
+          <t>13%</t>
+        </is>
+      </c>
+      <c r="V42" t="inlineStr">
+        <is>
+          <t>C:\Users\jonat\OneDrive\Escritorio\Repositorio\jonatha1992\Predictor_App\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W42" t="inlineStr"/>
+      <c r="X42" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y42" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2024-10-19 00:30:29</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr"/>
+      <c r="C43" t="n">
+        <v>13</v>
+      </c>
+      <c r="D43" t="n">
+        <v>4</v>
+      </c>
+      <c r="E43" t="n">
+        <v>9</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="inlineStr"/>
+      <c r="K43" t="inlineStr"/>
+      <c r="L43" t="inlineStr"/>
+      <c r="M43" t="inlineStr"/>
+      <c r="N43" t="n">
+        <v>10</v>
+      </c>
+      <c r="O43" t="n">
+        <v>10</v>
+      </c>
+      <c r="P43" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q43" t="inlineStr"/>
+      <c r="R43" t="n">
+        <v>5</v>
+      </c>
+      <c r="S43" t="inlineStr"/>
+      <c r="T43" t="n">
+        <v>20</v>
+      </c>
+      <c r="U43" t="inlineStr">
+        <is>
+          <t>34%</t>
+        </is>
+      </c>
+      <c r="V43" t="inlineStr">
+        <is>
+          <t>C:\Users\jonat\OneDrive\Escritorio\Repositorio\jonatha1992\Predictor_App\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W43" t="inlineStr"/>
+      <c r="X43" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y43" t="n">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
pruebas de lstm con 50 % de probabilidad al 20 umbral con cambiosn en los parametros de gru
</commit_message>
<xml_diff>
--- a/Data/Reporte_juego.xlsx
+++ b/Data/Reporte_juego.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y43"/>
+  <dimension ref="A1:Y44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3380,6 +3380,73 @@
         <v>38</v>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2024-10-20 01:59:54</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr"/>
+      <c r="C44" t="n">
+        <v>12</v>
+      </c>
+      <c r="D44" t="n">
+        <v>1</v>
+      </c>
+      <c r="E44" t="n">
+        <v>3</v>
+      </c>
+      <c r="F44" t="n">
+        <v>8</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" t="inlineStr"/>
+      <c r="J44" t="inlineStr"/>
+      <c r="K44" t="inlineStr"/>
+      <c r="L44" t="inlineStr"/>
+      <c r="M44" t="inlineStr"/>
+      <c r="N44" t="n">
+        <v>10</v>
+      </c>
+      <c r="O44" t="n">
+        <v>10</v>
+      </c>
+      <c r="P44" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q44" t="inlineStr"/>
+      <c r="R44" t="n">
+        <v>5</v>
+      </c>
+      <c r="S44" t="inlineStr"/>
+      <c r="T44" t="n">
+        <v>20</v>
+      </c>
+      <c r="U44" t="inlineStr">
+        <is>
+          <t>55%</t>
+        </is>
+      </c>
+      <c r="V44" t="inlineStr">
+        <is>
+          <t>C:\Users\jonat\OneDrive\Escritorio\Repositorio\jonatha1992\Predictor_App\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W44" t="inlineStr"/>
+      <c r="X44" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y44" t="n">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
colocacion de color par y vecinos para la prrediccion
</commit_message>
<xml_diff>
--- a/Data/Reporte_juego.xlsx
+++ b/Data/Reporte_juego.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y44"/>
+  <dimension ref="A1:Y69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3447,6 +3447,1681 @@
         <v>22</v>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2024-11-05 18:20:33</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr"/>
+      <c r="C45" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" t="inlineStr"/>
+      <c r="J45" t="inlineStr"/>
+      <c r="K45" t="inlineStr"/>
+      <c r="L45" t="inlineStr"/>
+      <c r="M45" t="inlineStr"/>
+      <c r="N45" t="n">
+        <v>10</v>
+      </c>
+      <c r="O45" t="n">
+        <v>4</v>
+      </c>
+      <c r="P45" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q45" t="inlineStr"/>
+      <c r="R45" t="n">
+        <v>5</v>
+      </c>
+      <c r="S45" t="inlineStr"/>
+      <c r="T45" t="n">
+        <v>20</v>
+      </c>
+      <c r="U45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V45" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Crupier.xlsx</t>
+        </is>
+      </c>
+      <c r="W45" t="inlineStr"/>
+      <c r="X45" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y45" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2024-11-05 18:23:21</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr"/>
+      <c r="C46" t="n">
+        <v>3</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" t="n">
+        <v>2</v>
+      </c>
+      <c r="F46" t="n">
+        <v>1</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" t="inlineStr"/>
+      <c r="J46" t="inlineStr"/>
+      <c r="K46" t="inlineStr"/>
+      <c r="L46" t="inlineStr"/>
+      <c r="M46" t="inlineStr"/>
+      <c r="N46" t="n">
+        <v>10</v>
+      </c>
+      <c r="O46" t="n">
+        <v>4</v>
+      </c>
+      <c r="P46" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q46" t="inlineStr"/>
+      <c r="R46" t="n">
+        <v>5</v>
+      </c>
+      <c r="S46" t="inlineStr"/>
+      <c r="T46" t="n">
+        <v>20</v>
+      </c>
+      <c r="U46" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="V46" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W46" t="inlineStr"/>
+      <c r="X46" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y46" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2024-11-05 18:24:51</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr"/>
+      <c r="C47" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0</v>
+      </c>
+      <c r="I47" t="inlineStr"/>
+      <c r="J47" t="inlineStr"/>
+      <c r="K47" t="inlineStr"/>
+      <c r="L47" t="inlineStr"/>
+      <c r="M47" t="inlineStr"/>
+      <c r="N47" t="n">
+        <v>10</v>
+      </c>
+      <c r="O47" t="n">
+        <v>4</v>
+      </c>
+      <c r="P47" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q47" t="inlineStr"/>
+      <c r="R47" t="n">
+        <v>5</v>
+      </c>
+      <c r="S47" t="inlineStr"/>
+      <c r="T47" t="n">
+        <v>20</v>
+      </c>
+      <c r="U47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V47" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W47" t="inlineStr"/>
+      <c r="X47" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2024-11-05 18:28:12</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr"/>
+      <c r="C48" t="n">
+        <v>1</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" t="n">
+        <v>1</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0</v>
+      </c>
+      <c r="I48" t="inlineStr"/>
+      <c r="J48" t="inlineStr"/>
+      <c r="K48" t="inlineStr"/>
+      <c r="L48" t="inlineStr"/>
+      <c r="M48" t="inlineStr"/>
+      <c r="N48" t="n">
+        <v>10</v>
+      </c>
+      <c r="O48" t="n">
+        <v>4</v>
+      </c>
+      <c r="P48" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q48" t="inlineStr"/>
+      <c r="R48" t="n">
+        <v>5</v>
+      </c>
+      <c r="S48" t="inlineStr"/>
+      <c r="T48" t="n">
+        <v>20</v>
+      </c>
+      <c r="U48" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="V48" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W48" t="inlineStr"/>
+      <c r="X48" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y48" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2024-11-05 18:30:27</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr"/>
+      <c r="C49" t="n">
+        <v>20</v>
+      </c>
+      <c r="D49" t="n">
+        <v>4</v>
+      </c>
+      <c r="E49" t="n">
+        <v>7</v>
+      </c>
+      <c r="F49" t="n">
+        <v>9</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I49" t="inlineStr"/>
+      <c r="J49" t="inlineStr"/>
+      <c r="K49" t="inlineStr"/>
+      <c r="L49" t="inlineStr"/>
+      <c r="M49" t="inlineStr"/>
+      <c r="N49" t="n">
+        <v>10</v>
+      </c>
+      <c r="O49" t="n">
+        <v>4</v>
+      </c>
+      <c r="P49" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q49" t="inlineStr"/>
+      <c r="R49" t="n">
+        <v>5</v>
+      </c>
+      <c r="S49" t="inlineStr"/>
+      <c r="T49" t="n">
+        <v>10</v>
+      </c>
+      <c r="U49" t="inlineStr">
+        <is>
+          <t>62%</t>
+        </is>
+      </c>
+      <c r="V49" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W49" t="inlineStr"/>
+      <c r="X49" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y49" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2024-11-05 18:32:11</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr"/>
+      <c r="C50" t="n">
+        <v>1</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" t="n">
+        <v>1</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0</v>
+      </c>
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="inlineStr"/>
+      <c r="K50" t="inlineStr"/>
+      <c r="L50" t="inlineStr"/>
+      <c r="M50" t="inlineStr"/>
+      <c r="N50" t="n">
+        <v>10</v>
+      </c>
+      <c r="O50" t="n">
+        <v>4</v>
+      </c>
+      <c r="P50" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q50" t="inlineStr"/>
+      <c r="R50" t="n">
+        <v>5</v>
+      </c>
+      <c r="S50" t="inlineStr"/>
+      <c r="T50" t="n">
+        <v>20</v>
+      </c>
+      <c r="U50" t="inlineStr">
+        <is>
+          <t>50%</t>
+        </is>
+      </c>
+      <c r="V50" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W50" t="inlineStr"/>
+      <c r="X50" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y50" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2024-11-06 19:17:34</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr"/>
+      <c r="C51" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0</v>
+      </c>
+      <c r="I51" t="inlineStr"/>
+      <c r="J51" t="inlineStr"/>
+      <c r="K51" t="inlineStr"/>
+      <c r="L51" t="inlineStr"/>
+      <c r="M51" t="inlineStr"/>
+      <c r="N51" t="n">
+        <v>10</v>
+      </c>
+      <c r="O51" t="n">
+        <v>4</v>
+      </c>
+      <c r="P51" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q51" t="inlineStr"/>
+      <c r="R51" t="n">
+        <v>7</v>
+      </c>
+      <c r="S51" t="inlineStr"/>
+      <c r="T51" t="n">
+        <v>50</v>
+      </c>
+      <c r="U51" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V51" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W51" t="inlineStr"/>
+      <c r="X51" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y51" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2024-11-07 18:56:39</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr"/>
+      <c r="C52" t="n">
+        <v>0</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" t="n">
+        <v>0</v>
+      </c>
+      <c r="H52" t="n">
+        <v>0</v>
+      </c>
+      <c r="I52" t="inlineStr"/>
+      <c r="J52" t="inlineStr"/>
+      <c r="K52" t="inlineStr"/>
+      <c r="L52" t="inlineStr"/>
+      <c r="M52" t="inlineStr"/>
+      <c r="N52" t="n">
+        <v>10</v>
+      </c>
+      <c r="O52" t="n">
+        <v>4</v>
+      </c>
+      <c r="P52" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q52" t="inlineStr"/>
+      <c r="R52" t="n">
+        <v>5</v>
+      </c>
+      <c r="S52" t="inlineStr"/>
+      <c r="T52" t="n">
+        <v>10</v>
+      </c>
+      <c r="U52" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V52" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W52" t="inlineStr"/>
+      <c r="X52" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y52" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2024-11-07 23:28:11</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr"/>
+      <c r="C53" t="n">
+        <v>42</v>
+      </c>
+      <c r="D53" t="n">
+        <v>11</v>
+      </c>
+      <c r="E53" t="n">
+        <v>31</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0</v>
+      </c>
+      <c r="H53" t="n">
+        <v>0</v>
+      </c>
+      <c r="I53" t="inlineStr"/>
+      <c r="J53" t="inlineStr"/>
+      <c r="K53" t="inlineStr"/>
+      <c r="L53" t="inlineStr"/>
+      <c r="M53" t="inlineStr"/>
+      <c r="N53" t="n">
+        <v>10</v>
+      </c>
+      <c r="O53" t="n">
+        <v>4</v>
+      </c>
+      <c r="P53" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q53" t="inlineStr"/>
+      <c r="R53" t="n">
+        <v>7</v>
+      </c>
+      <c r="S53" t="inlineStr"/>
+      <c r="T53" t="n">
+        <v>10</v>
+      </c>
+      <c r="U53" t="inlineStr">
+        <is>
+          <t>49%</t>
+        </is>
+      </c>
+      <c r="V53" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W53" t="inlineStr"/>
+      <c r="X53" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y53" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2024-11-08 06:41:49</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr"/>
+      <c r="C54" t="n">
+        <v>0</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0</v>
+      </c>
+      <c r="H54" t="n">
+        <v>0</v>
+      </c>
+      <c r="I54" t="inlineStr"/>
+      <c r="J54" t="inlineStr"/>
+      <c r="K54" t="inlineStr"/>
+      <c r="L54" t="inlineStr"/>
+      <c r="M54" t="inlineStr"/>
+      <c r="N54" t="n">
+        <v>10</v>
+      </c>
+      <c r="O54" t="n">
+        <v>4</v>
+      </c>
+      <c r="P54" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q54" t="inlineStr"/>
+      <c r="R54" t="n">
+        <v>7</v>
+      </c>
+      <c r="S54" t="inlineStr"/>
+      <c r="T54" t="n">
+        <v>10</v>
+      </c>
+      <c r="U54" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V54" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W54" t="inlineStr"/>
+      <c r="X54" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y54" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2024-11-09 13:58:57</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr"/>
+      <c r="C55" t="n">
+        <v>4</v>
+      </c>
+      <c r="D55" t="n">
+        <v>4</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0</v>
+      </c>
+      <c r="I55" t="inlineStr"/>
+      <c r="J55" t="inlineStr"/>
+      <c r="K55" t="inlineStr"/>
+      <c r="L55" t="inlineStr"/>
+      <c r="M55" t="inlineStr"/>
+      <c r="N55" t="n">
+        <v>10</v>
+      </c>
+      <c r="O55" t="n">
+        <v>4</v>
+      </c>
+      <c r="P55" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q55" t="inlineStr"/>
+      <c r="R55" t="n">
+        <v>10</v>
+      </c>
+      <c r="S55" t="inlineStr"/>
+      <c r="T55" t="n">
+        <v>5</v>
+      </c>
+      <c r="U55" t="inlineStr">
+        <is>
+          <t>18%</t>
+        </is>
+      </c>
+      <c r="V55" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Crupier.xlsx</t>
+        </is>
+      </c>
+      <c r="W55" t="inlineStr"/>
+      <c r="X55" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y55" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2024-11-09 13:59:06</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr"/>
+      <c r="C56" t="n">
+        <v>0</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0</v>
+      </c>
+      <c r="I56" t="inlineStr"/>
+      <c r="J56" t="inlineStr"/>
+      <c r="K56" t="inlineStr"/>
+      <c r="L56" t="inlineStr"/>
+      <c r="M56" t="inlineStr"/>
+      <c r="N56" t="n">
+        <v>10</v>
+      </c>
+      <c r="O56" t="n">
+        <v>4</v>
+      </c>
+      <c r="P56" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q56" t="inlineStr"/>
+      <c r="R56" t="n">
+        <v>10</v>
+      </c>
+      <c r="S56" t="inlineStr"/>
+      <c r="T56" t="n">
+        <v>5</v>
+      </c>
+      <c r="U56" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V56" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Crupier.xlsx</t>
+        </is>
+      </c>
+      <c r="W56" t="inlineStr"/>
+      <c r="X56" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2024-11-09 17:00:29</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr"/>
+      <c r="C57" t="n">
+        <v>2</v>
+      </c>
+      <c r="D57" t="n">
+        <v>2</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" t="n">
+        <v>0</v>
+      </c>
+      <c r="H57" t="n">
+        <v>0</v>
+      </c>
+      <c r="I57" t="inlineStr"/>
+      <c r="J57" t="inlineStr"/>
+      <c r="K57" t="inlineStr"/>
+      <c r="L57" t="inlineStr"/>
+      <c r="M57" t="inlineStr"/>
+      <c r="N57" t="n">
+        <v>10</v>
+      </c>
+      <c r="O57" t="n">
+        <v>8</v>
+      </c>
+      <c r="P57" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q57" t="inlineStr"/>
+      <c r="R57" t="n">
+        <v>5</v>
+      </c>
+      <c r="S57" t="inlineStr"/>
+      <c r="T57" t="n">
+        <v>10</v>
+      </c>
+      <c r="U57" t="inlineStr">
+        <is>
+          <t>9%</t>
+        </is>
+      </c>
+      <c r="V57" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W57" t="inlineStr"/>
+      <c r="X57" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y57" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2024-11-09 17:04:11</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr"/>
+      <c r="C58" t="n">
+        <v>6</v>
+      </c>
+      <c r="D58" t="n">
+        <v>3</v>
+      </c>
+      <c r="E58" t="n">
+        <v>3</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0</v>
+      </c>
+      <c r="I58" t="inlineStr"/>
+      <c r="J58" t="inlineStr"/>
+      <c r="K58" t="inlineStr"/>
+      <c r="L58" t="inlineStr"/>
+      <c r="M58" t="inlineStr"/>
+      <c r="N58" t="n">
+        <v>10</v>
+      </c>
+      <c r="O58" t="n">
+        <v>8</v>
+      </c>
+      <c r="P58" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q58" t="inlineStr"/>
+      <c r="R58" t="n">
+        <v>5</v>
+      </c>
+      <c r="S58" t="inlineStr"/>
+      <c r="T58" t="n">
+        <v>15</v>
+      </c>
+      <c r="U58" t="inlineStr">
+        <is>
+          <t>32%</t>
+        </is>
+      </c>
+      <c r="V58" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W58" t="inlineStr"/>
+      <c r="X58" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y58" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2024-11-09 17:05:03</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr"/>
+      <c r="C59" t="n">
+        <v>0</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0</v>
+      </c>
+      <c r="I59" t="inlineStr"/>
+      <c r="J59" t="inlineStr"/>
+      <c r="K59" t="inlineStr"/>
+      <c r="L59" t="inlineStr"/>
+      <c r="M59" t="inlineStr"/>
+      <c r="N59" t="n">
+        <v>10</v>
+      </c>
+      <c r="O59" t="n">
+        <v>8</v>
+      </c>
+      <c r="P59" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q59" t="inlineStr"/>
+      <c r="R59" t="n">
+        <v>5</v>
+      </c>
+      <c r="S59" t="inlineStr"/>
+      <c r="T59" t="n">
+        <v>20</v>
+      </c>
+      <c r="U59" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V59" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W59" t="inlineStr"/>
+      <c r="X59" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y59" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2024-11-09 17:06:24</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr"/>
+      <c r="C60" t="n">
+        <v>2</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0</v>
+      </c>
+      <c r="E60" t="n">
+        <v>1</v>
+      </c>
+      <c r="F60" t="n">
+        <v>1</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0</v>
+      </c>
+      <c r="I60" t="inlineStr"/>
+      <c r="J60" t="inlineStr"/>
+      <c r="K60" t="inlineStr"/>
+      <c r="L60" t="inlineStr"/>
+      <c r="M60" t="inlineStr"/>
+      <c r="N60" t="n">
+        <v>10</v>
+      </c>
+      <c r="O60" t="n">
+        <v>8</v>
+      </c>
+      <c r="P60" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q60" t="inlineStr"/>
+      <c r="R60" t="n">
+        <v>5</v>
+      </c>
+      <c r="S60" t="inlineStr"/>
+      <c r="T60" t="n">
+        <v>20</v>
+      </c>
+      <c r="U60" t="inlineStr">
+        <is>
+          <t>50%</t>
+        </is>
+      </c>
+      <c r="V60" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W60" t="inlineStr"/>
+      <c r="X60" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y60" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2024-11-09 17:07:12</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr"/>
+      <c r="C61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0</v>
+      </c>
+      <c r="F61" t="n">
+        <v>1</v>
+      </c>
+      <c r="G61" t="n">
+        <v>0</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0</v>
+      </c>
+      <c r="I61" t="inlineStr"/>
+      <c r="J61" t="inlineStr"/>
+      <c r="K61" t="inlineStr"/>
+      <c r="L61" t="inlineStr"/>
+      <c r="M61" t="inlineStr"/>
+      <c r="N61" t="n">
+        <v>10</v>
+      </c>
+      <c r="O61" t="n">
+        <v>8</v>
+      </c>
+      <c r="P61" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q61" t="inlineStr"/>
+      <c r="R61" t="n">
+        <v>5</v>
+      </c>
+      <c r="S61" t="inlineStr"/>
+      <c r="T61" t="n">
+        <v>20</v>
+      </c>
+      <c r="U61" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="V61" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W61" t="inlineStr"/>
+      <c r="X61" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y61" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2024-11-09 17:28:26</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr"/>
+      <c r="C62" t="n">
+        <v>3</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0</v>
+      </c>
+      <c r="E62" t="n">
+        <v>1</v>
+      </c>
+      <c r="F62" t="n">
+        <v>2</v>
+      </c>
+      <c r="G62" t="n">
+        <v>0</v>
+      </c>
+      <c r="H62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I62" t="inlineStr"/>
+      <c r="J62" t="inlineStr"/>
+      <c r="K62" t="inlineStr"/>
+      <c r="L62" t="inlineStr"/>
+      <c r="M62" t="inlineStr"/>
+      <c r="N62" t="n">
+        <v>10</v>
+      </c>
+      <c r="O62" t="n">
+        <v>3</v>
+      </c>
+      <c r="P62" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q62" t="inlineStr"/>
+      <c r="R62" t="n">
+        <v>1</v>
+      </c>
+      <c r="S62" t="inlineStr"/>
+      <c r="T62" t="n">
+        <v>10</v>
+      </c>
+      <c r="U62" t="inlineStr">
+        <is>
+          <t>15%</t>
+        </is>
+      </c>
+      <c r="V62" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W62" t="inlineStr"/>
+      <c r="X62" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y62" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2024-11-09 17:29:29</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr"/>
+      <c r="C63" t="n">
+        <v>0</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0</v>
+      </c>
+      <c r="G63" t="n">
+        <v>0</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0</v>
+      </c>
+      <c r="I63" t="inlineStr"/>
+      <c r="J63" t="inlineStr"/>
+      <c r="K63" t="inlineStr"/>
+      <c r="L63" t="inlineStr"/>
+      <c r="M63" t="inlineStr"/>
+      <c r="N63" t="n">
+        <v>10</v>
+      </c>
+      <c r="O63" t="n">
+        <v>3</v>
+      </c>
+      <c r="P63" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q63" t="inlineStr"/>
+      <c r="R63" t="n">
+        <v>1</v>
+      </c>
+      <c r="S63" t="inlineStr"/>
+      <c r="T63" t="n">
+        <v>10</v>
+      </c>
+      <c r="U63" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="V63" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W63" t="inlineStr"/>
+      <c r="X63" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y63" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2024-11-09 20:05:08</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr"/>
+      <c r="C64" t="n">
+        <v>11</v>
+      </c>
+      <c r="D64" t="n">
+        <v>4</v>
+      </c>
+      <c r="E64" t="n">
+        <v>4</v>
+      </c>
+      <c r="F64" t="n">
+        <v>3</v>
+      </c>
+      <c r="G64" t="n">
+        <v>0</v>
+      </c>
+      <c r="H64" t="n">
+        <v>0</v>
+      </c>
+      <c r="I64" t="inlineStr"/>
+      <c r="J64" t="inlineStr"/>
+      <c r="K64" t="inlineStr"/>
+      <c r="L64" t="inlineStr"/>
+      <c r="M64" t="inlineStr"/>
+      <c r="N64" t="n">
+        <v>10</v>
+      </c>
+      <c r="O64" t="n">
+        <v>3</v>
+      </c>
+      <c r="P64" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q64" t="inlineStr"/>
+      <c r="R64" t="n">
+        <v>3</v>
+      </c>
+      <c r="S64" t="inlineStr"/>
+      <c r="T64" t="n">
+        <v>10</v>
+      </c>
+      <c r="U64" t="inlineStr">
+        <is>
+          <t>41%</t>
+        </is>
+      </c>
+      <c r="V64" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W64" t="inlineStr"/>
+      <c r="X64" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y64" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2024-11-09 20:10:55</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr"/>
+      <c r="C65" t="n">
+        <v>16</v>
+      </c>
+      <c r="D65" t="n">
+        <v>5</v>
+      </c>
+      <c r="E65" t="n">
+        <v>4</v>
+      </c>
+      <c r="F65" t="n">
+        <v>7</v>
+      </c>
+      <c r="G65" t="n">
+        <v>0</v>
+      </c>
+      <c r="H65" t="n">
+        <v>0</v>
+      </c>
+      <c r="I65" t="inlineStr"/>
+      <c r="J65" t="inlineStr"/>
+      <c r="K65" t="inlineStr"/>
+      <c r="L65" t="inlineStr"/>
+      <c r="M65" t="inlineStr"/>
+      <c r="N65" t="n">
+        <v>10</v>
+      </c>
+      <c r="O65" t="n">
+        <v>3</v>
+      </c>
+      <c r="P65" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q65" t="inlineStr"/>
+      <c r="R65" t="n">
+        <v>3</v>
+      </c>
+      <c r="S65" t="inlineStr"/>
+      <c r="T65" t="n">
+        <v>10</v>
+      </c>
+      <c r="U65" t="inlineStr">
+        <is>
+          <t>32%</t>
+        </is>
+      </c>
+      <c r="V65" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W65" t="inlineStr"/>
+      <c r="X65" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y65" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2024-11-09 23:13:04</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr"/>
+      <c r="C66" t="n">
+        <v>0</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0</v>
+      </c>
+      <c r="G66" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" t="inlineStr"/>
+      <c r="J66" t="inlineStr"/>
+      <c r="K66" t="inlineStr"/>
+      <c r="L66" t="inlineStr"/>
+      <c r="M66" t="inlineStr"/>
+      <c r="N66" t="n">
+        <v>10</v>
+      </c>
+      <c r="O66" t="n">
+        <v>7</v>
+      </c>
+      <c r="P66" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q66" t="inlineStr"/>
+      <c r="R66" t="n">
+        <v>5</v>
+      </c>
+      <c r="S66" t="inlineStr"/>
+      <c r="T66" t="n">
+        <v>10</v>
+      </c>
+      <c r="U66" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="V66" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W66" t="inlineStr"/>
+      <c r="X66" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y66" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2024-11-10 17:26:44</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr"/>
+      <c r="C67" t="n">
+        <v>0</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0</v>
+      </c>
+      <c r="G67" t="n">
+        <v>0</v>
+      </c>
+      <c r="H67" t="n">
+        <v>0</v>
+      </c>
+      <c r="I67" t="inlineStr"/>
+      <c r="J67" t="inlineStr"/>
+      <c r="K67" t="inlineStr"/>
+      <c r="L67" t="inlineStr"/>
+      <c r="M67" t="inlineStr"/>
+      <c r="N67" t="n">
+        <v>10</v>
+      </c>
+      <c r="O67" t="n">
+        <v>7</v>
+      </c>
+      <c r="P67" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q67" t="inlineStr"/>
+      <c r="R67" t="n">
+        <v>5</v>
+      </c>
+      <c r="S67" t="inlineStr"/>
+      <c r="T67" t="n">
+        <v>10</v>
+      </c>
+      <c r="U67" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="V67" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W67" t="inlineStr"/>
+      <c r="X67" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y67" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2024-11-10 19:02:15</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr"/>
+      <c r="C68" t="n">
+        <v>8</v>
+      </c>
+      <c r="D68" t="n">
+        <v>3</v>
+      </c>
+      <c r="E68" t="n">
+        <v>5</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0</v>
+      </c>
+      <c r="G68" t="n">
+        <v>0</v>
+      </c>
+      <c r="H68" t="n">
+        <v>0</v>
+      </c>
+      <c r="I68" t="inlineStr"/>
+      <c r="J68" t="inlineStr"/>
+      <c r="K68" t="inlineStr"/>
+      <c r="L68" t="inlineStr"/>
+      <c r="M68" t="inlineStr"/>
+      <c r="N68" t="n">
+        <v>10</v>
+      </c>
+      <c r="O68" t="n">
+        <v>7</v>
+      </c>
+      <c r="P68" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q68" t="inlineStr"/>
+      <c r="R68" t="n">
+        <v>5</v>
+      </c>
+      <c r="S68" t="inlineStr"/>
+      <c r="T68" t="n">
+        <v>10</v>
+      </c>
+      <c r="U68" t="inlineStr">
+        <is>
+          <t>33%</t>
+        </is>
+      </c>
+      <c r="V68" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W68" t="inlineStr"/>
+      <c r="X68" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y68" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2024-11-10 19:54:07</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr"/>
+      <c r="C69" t="n">
+        <v>46</v>
+      </c>
+      <c r="D69" t="n">
+        <v>8</v>
+      </c>
+      <c r="E69" t="n">
+        <v>14</v>
+      </c>
+      <c r="F69" t="n">
+        <v>24</v>
+      </c>
+      <c r="G69" t="n">
+        <v>0</v>
+      </c>
+      <c r="H69" t="n">
+        <v>0</v>
+      </c>
+      <c r="I69" t="inlineStr"/>
+      <c r="J69" t="inlineStr"/>
+      <c r="K69" t="inlineStr"/>
+      <c r="L69" t="inlineStr"/>
+      <c r="M69" t="inlineStr"/>
+      <c r="N69" t="n">
+        <v>10</v>
+      </c>
+      <c r="O69" t="n">
+        <v>7</v>
+      </c>
+      <c r="P69" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q69" t="inlineStr"/>
+      <c r="R69" t="n">
+        <v>5</v>
+      </c>
+      <c r="S69" t="inlineStr"/>
+      <c r="T69" t="n">
+        <v>20</v>
+      </c>
+      <c r="U69" t="inlineStr">
+        <is>
+          <t>62%</t>
+        </is>
+      </c>
+      <c r="V69" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W69" t="inlineStr"/>
+      <c r="X69" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y69" t="n">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
eliminacion  de codigo innecesario y tambien  se tiene que verificar por que no pego ninguno
</commit_message>
<xml_diff>
--- a/Data/Reporte_juego.xlsx
+++ b/Data/Reporte_juego.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y69"/>
+  <dimension ref="A1:Y89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5122,6 +5122,1346 @@
         <v>74</v>
       </c>
     </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2024-11-16 17:51:56</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr"/>
+      <c r="C70" t="n">
+        <v>21</v>
+      </c>
+      <c r="D70" t="n">
+        <v>2</v>
+      </c>
+      <c r="E70" t="n">
+        <v>10</v>
+      </c>
+      <c r="F70" t="n">
+        <v>9</v>
+      </c>
+      <c r="G70" t="n">
+        <v>0</v>
+      </c>
+      <c r="H70" t="n">
+        <v>0</v>
+      </c>
+      <c r="I70" t="inlineStr"/>
+      <c r="J70" t="inlineStr"/>
+      <c r="K70" t="inlineStr"/>
+      <c r="L70" t="inlineStr"/>
+      <c r="M70" t="inlineStr"/>
+      <c r="N70" t="n">
+        <v>10</v>
+      </c>
+      <c r="O70" t="n">
+        <v>7</v>
+      </c>
+      <c r="P70" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q70" t="inlineStr"/>
+      <c r="R70" t="n">
+        <v>5</v>
+      </c>
+      <c r="S70" t="inlineStr"/>
+      <c r="T70" t="n">
+        <v>20</v>
+      </c>
+      <c r="U70" t="inlineStr">
+        <is>
+          <t>70%</t>
+        </is>
+      </c>
+      <c r="V70" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W70" t="inlineStr"/>
+      <c r="X70" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y70" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2024-11-16 17:54:03</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr"/>
+      <c r="C71" t="n">
+        <v>16</v>
+      </c>
+      <c r="D71" t="n">
+        <v>2</v>
+      </c>
+      <c r="E71" t="n">
+        <v>8</v>
+      </c>
+      <c r="F71" t="n">
+        <v>6</v>
+      </c>
+      <c r="G71" t="n">
+        <v>0</v>
+      </c>
+      <c r="H71" t="n">
+        <v>0</v>
+      </c>
+      <c r="I71" t="inlineStr"/>
+      <c r="J71" t="inlineStr"/>
+      <c r="K71" t="inlineStr"/>
+      <c r="L71" t="inlineStr"/>
+      <c r="M71" t="inlineStr"/>
+      <c r="N71" t="n">
+        <v>10</v>
+      </c>
+      <c r="O71" t="n">
+        <v>7</v>
+      </c>
+      <c r="P71" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q71" t="inlineStr"/>
+      <c r="R71" t="n">
+        <v>5</v>
+      </c>
+      <c r="S71" t="inlineStr"/>
+      <c r="T71" t="n">
+        <v>20</v>
+      </c>
+      <c r="U71" t="inlineStr">
+        <is>
+          <t>70%</t>
+        </is>
+      </c>
+      <c r="V71" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W71" t="inlineStr"/>
+      <c r="X71" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y71" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2024-11-17 11:18:02</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr"/>
+      <c r="C72" t="n">
+        <v>0</v>
+      </c>
+      <c r="D72" t="n">
+        <v>0</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0</v>
+      </c>
+      <c r="G72" t="n">
+        <v>0</v>
+      </c>
+      <c r="H72" t="n">
+        <v>0</v>
+      </c>
+      <c r="I72" t="inlineStr"/>
+      <c r="J72" t="inlineStr"/>
+      <c r="K72" t="inlineStr"/>
+      <c r="L72" t="inlineStr"/>
+      <c r="M72" t="inlineStr"/>
+      <c r="N72" t="n">
+        <v>10</v>
+      </c>
+      <c r="O72" t="n">
+        <v>7</v>
+      </c>
+      <c r="P72" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q72" t="inlineStr"/>
+      <c r="R72" t="n">
+        <v>3</v>
+      </c>
+      <c r="S72" t="inlineStr"/>
+      <c r="T72" t="n">
+        <v>20</v>
+      </c>
+      <c r="U72" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V72" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W72" t="inlineStr"/>
+      <c r="X72" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y72" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2024-11-17 11:27:53</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr"/>
+      <c r="C73" t="n">
+        <v>29</v>
+      </c>
+      <c r="D73" t="n">
+        <v>8</v>
+      </c>
+      <c r="E73" t="n">
+        <v>21</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0</v>
+      </c>
+      <c r="G73" t="n">
+        <v>0</v>
+      </c>
+      <c r="H73" t="n">
+        <v>0</v>
+      </c>
+      <c r="I73" t="inlineStr"/>
+      <c r="J73" t="inlineStr"/>
+      <c r="K73" t="inlineStr"/>
+      <c r="L73" t="inlineStr"/>
+      <c r="M73" t="inlineStr"/>
+      <c r="N73" t="n">
+        <v>10</v>
+      </c>
+      <c r="O73" t="n">
+        <v>7</v>
+      </c>
+      <c r="P73" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q73" t="inlineStr"/>
+      <c r="R73" t="n">
+        <v>3</v>
+      </c>
+      <c r="S73" t="inlineStr"/>
+      <c r="T73" t="n">
+        <v>20</v>
+      </c>
+      <c r="U73" t="inlineStr">
+        <is>
+          <t>29%</t>
+        </is>
+      </c>
+      <c r="V73" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W73" t="inlineStr"/>
+      <c r="X73" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y73" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2024-11-17 11:28:06</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr"/>
+      <c r="C74" t="n">
+        <v>0</v>
+      </c>
+      <c r="D74" t="n">
+        <v>0</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0</v>
+      </c>
+      <c r="G74" t="n">
+        <v>0</v>
+      </c>
+      <c r="H74" t="n">
+        <v>0</v>
+      </c>
+      <c r="I74" t="inlineStr"/>
+      <c r="J74" t="inlineStr"/>
+      <c r="K74" t="inlineStr"/>
+      <c r="L74" t="inlineStr"/>
+      <c r="M74" t="inlineStr"/>
+      <c r="N74" t="n">
+        <v>10</v>
+      </c>
+      <c r="O74" t="n">
+        <v>7</v>
+      </c>
+      <c r="P74" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q74" t="inlineStr"/>
+      <c r="R74" t="n">
+        <v>1</v>
+      </c>
+      <c r="S74" t="inlineStr"/>
+      <c r="T74" t="n">
+        <v>30</v>
+      </c>
+      <c r="U74" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V74" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W74" t="inlineStr"/>
+      <c r="X74" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y74" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2024-11-17 11:28:42</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr"/>
+      <c r="C75" t="n">
+        <v>0</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0</v>
+      </c>
+      <c r="G75" t="n">
+        <v>0</v>
+      </c>
+      <c r="H75" t="n">
+        <v>0</v>
+      </c>
+      <c r="I75" t="inlineStr"/>
+      <c r="J75" t="inlineStr"/>
+      <c r="K75" t="inlineStr"/>
+      <c r="L75" t="inlineStr"/>
+      <c r="M75" t="inlineStr"/>
+      <c r="N75" t="n">
+        <v>10</v>
+      </c>
+      <c r="O75" t="n">
+        <v>7</v>
+      </c>
+      <c r="P75" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q75" t="inlineStr"/>
+      <c r="R75" t="n">
+        <v>1</v>
+      </c>
+      <c r="S75" t="inlineStr"/>
+      <c r="T75" t="n">
+        <v>30</v>
+      </c>
+      <c r="U75" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="V75" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W75" t="inlineStr"/>
+      <c r="X75" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y75" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2024-11-17 16:08:21</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr"/>
+      <c r="C76" t="n">
+        <v>18</v>
+      </c>
+      <c r="D76" t="n">
+        <v>3</v>
+      </c>
+      <c r="E76" t="n">
+        <v>9</v>
+      </c>
+      <c r="F76" t="n">
+        <v>6</v>
+      </c>
+      <c r="G76" t="n">
+        <v>0</v>
+      </c>
+      <c r="H76" t="n">
+        <v>0</v>
+      </c>
+      <c r="I76" t="inlineStr"/>
+      <c r="J76" t="inlineStr"/>
+      <c r="K76" t="inlineStr"/>
+      <c r="L76" t="inlineStr"/>
+      <c r="M76" t="inlineStr"/>
+      <c r="N76" t="n">
+        <v>10</v>
+      </c>
+      <c r="O76" t="n">
+        <v>7</v>
+      </c>
+      <c r="P76" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q76" t="inlineStr"/>
+      <c r="R76" t="n">
+        <v>3</v>
+      </c>
+      <c r="S76" t="inlineStr"/>
+      <c r="T76" t="n">
+        <v>40</v>
+      </c>
+      <c r="U76" t="inlineStr">
+        <is>
+          <t>40%</t>
+        </is>
+      </c>
+      <c r="V76" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W76" t="inlineStr"/>
+      <c r="X76" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y76" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2024-11-18 14:56:44</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr"/>
+      <c r="C77" t="n">
+        <v>0</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0</v>
+      </c>
+      <c r="G77" t="n">
+        <v>0</v>
+      </c>
+      <c r="H77" t="n">
+        <v>0</v>
+      </c>
+      <c r="I77" t="inlineStr"/>
+      <c r="J77" t="inlineStr"/>
+      <c r="K77" t="inlineStr"/>
+      <c r="L77" t="inlineStr"/>
+      <c r="M77" t="inlineStr"/>
+      <c r="N77" t="n">
+        <v>10</v>
+      </c>
+      <c r="O77" t="n">
+        <v>7</v>
+      </c>
+      <c r="P77" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q77" t="inlineStr"/>
+      <c r="R77" t="n">
+        <v>5</v>
+      </c>
+      <c r="S77" t="inlineStr"/>
+      <c r="T77" t="n">
+        <v>40</v>
+      </c>
+      <c r="U77" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V77" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W77" t="inlineStr"/>
+      <c r="X77" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y77" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2024-11-18 14:58:36</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr"/>
+      <c r="C78" t="n">
+        <v>3</v>
+      </c>
+      <c r="D78" t="n">
+        <v>0</v>
+      </c>
+      <c r="E78" t="n">
+        <v>2</v>
+      </c>
+      <c r="F78" t="n">
+        <v>1</v>
+      </c>
+      <c r="G78" t="n">
+        <v>0</v>
+      </c>
+      <c r="H78" t="n">
+        <v>0</v>
+      </c>
+      <c r="I78" t="inlineStr"/>
+      <c r="J78" t="inlineStr"/>
+      <c r="K78" t="inlineStr"/>
+      <c r="L78" t="inlineStr"/>
+      <c r="M78" t="inlineStr"/>
+      <c r="N78" t="n">
+        <v>10</v>
+      </c>
+      <c r="O78" t="n">
+        <v>7</v>
+      </c>
+      <c r="P78" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q78" t="inlineStr"/>
+      <c r="R78" t="n">
+        <v>5</v>
+      </c>
+      <c r="S78" t="inlineStr"/>
+      <c r="T78" t="n">
+        <v>50</v>
+      </c>
+      <c r="U78" t="inlineStr">
+        <is>
+          <t>38%</t>
+        </is>
+      </c>
+      <c r="V78" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W78" t="inlineStr"/>
+      <c r="X78" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y78" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2024-11-18 14:58:54</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr"/>
+      <c r="C79" t="n">
+        <v>0</v>
+      </c>
+      <c r="D79" t="n">
+        <v>0</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0</v>
+      </c>
+      <c r="G79" t="n">
+        <v>0</v>
+      </c>
+      <c r="H79" t="n">
+        <v>0</v>
+      </c>
+      <c r="I79" t="inlineStr"/>
+      <c r="J79" t="inlineStr"/>
+      <c r="K79" t="inlineStr"/>
+      <c r="L79" t="inlineStr"/>
+      <c r="M79" t="inlineStr"/>
+      <c r="N79" t="n">
+        <v>10</v>
+      </c>
+      <c r="O79" t="n">
+        <v>7</v>
+      </c>
+      <c r="P79" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q79" t="inlineStr"/>
+      <c r="R79" t="n">
+        <v>5</v>
+      </c>
+      <c r="S79" t="inlineStr"/>
+      <c r="T79" t="n">
+        <v>40</v>
+      </c>
+      <c r="U79" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V79" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W79" t="inlineStr"/>
+      <c r="X79" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y79" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2024-11-18 15:00:51</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr"/>
+      <c r="C80" t="n">
+        <v>10</v>
+      </c>
+      <c r="D80" t="n">
+        <v>3</v>
+      </c>
+      <c r="E80" t="n">
+        <v>3</v>
+      </c>
+      <c r="F80" t="n">
+        <v>4</v>
+      </c>
+      <c r="G80" t="n">
+        <v>0</v>
+      </c>
+      <c r="H80" t="n">
+        <v>0</v>
+      </c>
+      <c r="I80" t="inlineStr"/>
+      <c r="J80" t="inlineStr"/>
+      <c r="K80" t="inlineStr"/>
+      <c r="L80" t="inlineStr"/>
+      <c r="M80" t="inlineStr"/>
+      <c r="N80" t="n">
+        <v>10</v>
+      </c>
+      <c r="O80" t="n">
+        <v>7</v>
+      </c>
+      <c r="P80" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q80" t="inlineStr"/>
+      <c r="R80" t="n">
+        <v>5</v>
+      </c>
+      <c r="S80" t="inlineStr"/>
+      <c r="T80" t="n">
+        <v>40</v>
+      </c>
+      <c r="U80" t="inlineStr">
+        <is>
+          <t>53%</t>
+        </is>
+      </c>
+      <c r="V80" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W80" t="inlineStr"/>
+      <c r="X80" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y80" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2024-11-18 16:01:53</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr"/>
+      <c r="C81" t="n">
+        <v>11</v>
+      </c>
+      <c r="D81" t="n">
+        <v>3</v>
+      </c>
+      <c r="E81" t="n">
+        <v>5</v>
+      </c>
+      <c r="F81" t="n">
+        <v>3</v>
+      </c>
+      <c r="G81" t="n">
+        <v>0</v>
+      </c>
+      <c r="H81" t="n">
+        <v>0</v>
+      </c>
+      <c r="I81" t="inlineStr"/>
+      <c r="J81" t="inlineStr"/>
+      <c r="K81" t="inlineStr"/>
+      <c r="L81" t="inlineStr"/>
+      <c r="M81" t="inlineStr"/>
+      <c r="N81" t="n">
+        <v>10</v>
+      </c>
+      <c r="O81" t="n">
+        <v>7</v>
+      </c>
+      <c r="P81" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q81" t="inlineStr"/>
+      <c r="R81" t="n">
+        <v>5</v>
+      </c>
+      <c r="S81" t="inlineStr"/>
+      <c r="T81" t="n">
+        <v>50</v>
+      </c>
+      <c r="U81" t="inlineStr">
+        <is>
+          <t>46%</t>
+        </is>
+      </c>
+      <c r="V81" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W81" t="inlineStr"/>
+      <c r="X81" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y81" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2024-11-18 16:04:25</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr"/>
+      <c r="C82" t="n">
+        <v>13</v>
+      </c>
+      <c r="D82" t="n">
+        <v>2</v>
+      </c>
+      <c r="E82" t="n">
+        <v>3</v>
+      </c>
+      <c r="F82" t="n">
+        <v>3</v>
+      </c>
+      <c r="G82" t="n">
+        <v>5</v>
+      </c>
+      <c r="H82" t="n">
+        <v>0</v>
+      </c>
+      <c r="I82" t="inlineStr"/>
+      <c r="J82" t="inlineStr"/>
+      <c r="K82" t="inlineStr"/>
+      <c r="L82" t="inlineStr"/>
+      <c r="M82" t="inlineStr"/>
+      <c r="N82" t="n">
+        <v>10</v>
+      </c>
+      <c r="O82" t="n">
+        <v>7</v>
+      </c>
+      <c r="P82" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q82" t="inlineStr"/>
+      <c r="R82" t="n">
+        <v>1</v>
+      </c>
+      <c r="S82" t="inlineStr"/>
+      <c r="T82" t="n">
+        <v>10</v>
+      </c>
+      <c r="U82" t="inlineStr">
+        <is>
+          <t>17%</t>
+        </is>
+      </c>
+      <c r="V82" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W82" t="inlineStr"/>
+      <c r="X82" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y82" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2024-11-18 16:04:47</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr"/>
+      <c r="C83" t="n">
+        <v>0</v>
+      </c>
+      <c r="D83" t="n">
+        <v>0</v>
+      </c>
+      <c r="E83" t="n">
+        <v>0</v>
+      </c>
+      <c r="F83" t="n">
+        <v>0</v>
+      </c>
+      <c r="G83" t="n">
+        <v>0</v>
+      </c>
+      <c r="H83" t="n">
+        <v>0</v>
+      </c>
+      <c r="I83" t="inlineStr"/>
+      <c r="J83" t="inlineStr"/>
+      <c r="K83" t="inlineStr"/>
+      <c r="L83" t="inlineStr"/>
+      <c r="M83" t="inlineStr"/>
+      <c r="N83" t="n">
+        <v>10</v>
+      </c>
+      <c r="O83" t="n">
+        <v>7</v>
+      </c>
+      <c r="P83" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q83" t="inlineStr"/>
+      <c r="R83" t="n">
+        <v>5</v>
+      </c>
+      <c r="S83" t="inlineStr"/>
+      <c r="T83" t="n">
+        <v>10</v>
+      </c>
+      <c r="U83" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V83" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W83" t="inlineStr"/>
+      <c r="X83" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y83" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2024-11-18 16:06:56</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr"/>
+      <c r="C84" t="n">
+        <v>7</v>
+      </c>
+      <c r="D84" t="n">
+        <v>2</v>
+      </c>
+      <c r="E84" t="n">
+        <v>5</v>
+      </c>
+      <c r="F84" t="n">
+        <v>0</v>
+      </c>
+      <c r="G84" t="n">
+        <v>0</v>
+      </c>
+      <c r="H84" t="n">
+        <v>0</v>
+      </c>
+      <c r="I84" t="inlineStr"/>
+      <c r="J84" t="inlineStr"/>
+      <c r="K84" t="inlineStr"/>
+      <c r="L84" t="inlineStr"/>
+      <c r="M84" t="inlineStr"/>
+      <c r="N84" t="n">
+        <v>10</v>
+      </c>
+      <c r="O84" t="n">
+        <v>7</v>
+      </c>
+      <c r="P84" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q84" t="inlineStr"/>
+      <c r="R84" t="n">
+        <v>5</v>
+      </c>
+      <c r="S84" t="inlineStr"/>
+      <c r="T84" t="n">
+        <v>10</v>
+      </c>
+      <c r="U84" t="inlineStr">
+        <is>
+          <t>30%</t>
+        </is>
+      </c>
+      <c r="V84" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W84" t="inlineStr"/>
+      <c r="X84" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y84" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2024-11-18 20:16:32</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr"/>
+      <c r="C85" t="n">
+        <v>16</v>
+      </c>
+      <c r="D85" t="n">
+        <v>1</v>
+      </c>
+      <c r="E85" t="n">
+        <v>6</v>
+      </c>
+      <c r="F85" t="n">
+        <v>9</v>
+      </c>
+      <c r="G85" t="n">
+        <v>0</v>
+      </c>
+      <c r="H85" t="n">
+        <v>0</v>
+      </c>
+      <c r="I85" t="inlineStr"/>
+      <c r="J85" t="inlineStr"/>
+      <c r="K85" t="inlineStr"/>
+      <c r="L85" t="inlineStr"/>
+      <c r="M85" t="inlineStr"/>
+      <c r="N85" t="n">
+        <v>10</v>
+      </c>
+      <c r="O85" t="n">
+        <v>7</v>
+      </c>
+      <c r="P85" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q85" t="inlineStr"/>
+      <c r="R85" t="n">
+        <v>5</v>
+      </c>
+      <c r="S85" t="inlineStr"/>
+      <c r="T85" t="n">
+        <v>40</v>
+      </c>
+      <c r="U85" t="inlineStr">
+        <is>
+          <t>59%</t>
+        </is>
+      </c>
+      <c r="V85" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W85" t="inlineStr"/>
+      <c r="X85" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y85" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2024-11-18 21:13:48</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr"/>
+      <c r="C86" t="n">
+        <v>24</v>
+      </c>
+      <c r="D86" t="n">
+        <v>3</v>
+      </c>
+      <c r="E86" t="n">
+        <v>9</v>
+      </c>
+      <c r="F86" t="n">
+        <v>12</v>
+      </c>
+      <c r="G86" t="n">
+        <v>0</v>
+      </c>
+      <c r="H86" t="n">
+        <v>0</v>
+      </c>
+      <c r="I86" t="inlineStr"/>
+      <c r="J86" t="inlineStr"/>
+      <c r="K86" t="inlineStr"/>
+      <c r="L86" t="inlineStr"/>
+      <c r="M86" t="inlineStr"/>
+      <c r="N86" t="n">
+        <v>10</v>
+      </c>
+      <c r="O86" t="n">
+        <v>7</v>
+      </c>
+      <c r="P86" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q86" t="inlineStr"/>
+      <c r="R86" t="n">
+        <v>5</v>
+      </c>
+      <c r="S86" t="inlineStr"/>
+      <c r="T86" t="n">
+        <v>40</v>
+      </c>
+      <c r="U86" t="inlineStr">
+        <is>
+          <t>77%</t>
+        </is>
+      </c>
+      <c r="V86" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W86" t="inlineStr"/>
+      <c r="X86" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y86" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2024-11-18 23:22:05</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr"/>
+      <c r="C87" t="n">
+        <v>7</v>
+      </c>
+      <c r="D87" t="n">
+        <v>1</v>
+      </c>
+      <c r="E87" t="n">
+        <v>3</v>
+      </c>
+      <c r="F87" t="n">
+        <v>3</v>
+      </c>
+      <c r="G87" t="n">
+        <v>0</v>
+      </c>
+      <c r="H87" t="n">
+        <v>0</v>
+      </c>
+      <c r="I87" t="inlineStr"/>
+      <c r="J87" t="inlineStr"/>
+      <c r="K87" t="inlineStr"/>
+      <c r="L87" t="inlineStr"/>
+      <c r="M87" t="inlineStr"/>
+      <c r="N87" t="n">
+        <v>10</v>
+      </c>
+      <c r="O87" t="n">
+        <v>7</v>
+      </c>
+      <c r="P87" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q87" t="inlineStr"/>
+      <c r="R87" t="n">
+        <v>5</v>
+      </c>
+      <c r="S87" t="inlineStr"/>
+      <c r="T87" t="n">
+        <v>40</v>
+      </c>
+      <c r="U87" t="inlineStr">
+        <is>
+          <t>35%</t>
+        </is>
+      </c>
+      <c r="V87" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Crupier.xlsx</t>
+        </is>
+      </c>
+      <c r="W87" t="inlineStr"/>
+      <c r="X87" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y87" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2024-11-18 23:27:10</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr"/>
+      <c r="C88" t="n">
+        <v>13</v>
+      </c>
+      <c r="D88" t="n">
+        <v>0</v>
+      </c>
+      <c r="E88" t="n">
+        <v>7</v>
+      </c>
+      <c r="F88" t="n">
+        <v>6</v>
+      </c>
+      <c r="G88" t="n">
+        <v>0</v>
+      </c>
+      <c r="H88" t="n">
+        <v>0</v>
+      </c>
+      <c r="I88" t="inlineStr"/>
+      <c r="J88" t="inlineStr"/>
+      <c r="K88" t="inlineStr"/>
+      <c r="L88" t="inlineStr"/>
+      <c r="M88" t="inlineStr"/>
+      <c r="N88" t="n">
+        <v>10</v>
+      </c>
+      <c r="O88" t="n">
+        <v>7</v>
+      </c>
+      <c r="P88" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q88" t="inlineStr"/>
+      <c r="R88" t="n">
+        <v>5</v>
+      </c>
+      <c r="S88" t="inlineStr"/>
+      <c r="T88" t="n">
+        <v>20</v>
+      </c>
+      <c r="U88" t="inlineStr">
+        <is>
+          <t>48%</t>
+        </is>
+      </c>
+      <c r="V88" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Crupier.xlsx</t>
+        </is>
+      </c>
+      <c r="W88" t="inlineStr"/>
+      <c r="X88" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y88" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2024-11-18 23:28:03</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr"/>
+      <c r="C89" t="n">
+        <v>2</v>
+      </c>
+      <c r="D89" t="n">
+        <v>0</v>
+      </c>
+      <c r="E89" t="n">
+        <v>2</v>
+      </c>
+      <c r="F89" t="n">
+        <v>0</v>
+      </c>
+      <c r="G89" t="n">
+        <v>0</v>
+      </c>
+      <c r="H89" t="n">
+        <v>0</v>
+      </c>
+      <c r="I89" t="inlineStr"/>
+      <c r="J89" t="inlineStr"/>
+      <c r="K89" t="inlineStr"/>
+      <c r="L89" t="inlineStr"/>
+      <c r="M89" t="inlineStr"/>
+      <c r="N89" t="n">
+        <v>10</v>
+      </c>
+      <c r="O89" t="n">
+        <v>7</v>
+      </c>
+      <c r="P89" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q89" t="inlineStr"/>
+      <c r="R89" t="n">
+        <v>2</v>
+      </c>
+      <c r="S89" t="inlineStr"/>
+      <c r="T89" t="n">
+        <v>20</v>
+      </c>
+      <c r="U89" t="inlineStr">
+        <is>
+          <t>20%</t>
+        </is>
+      </c>
+      <c r="V89" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Crupier.xlsx</t>
+        </is>
+      </c>
+      <c r="W89" t="inlineStr"/>
+      <c r="X89" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y89" t="n">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
cambios en el historial de de los numero la eliminacion lo va a decir la probabilidad   0
</commit_message>
<xml_diff>
--- a/Data/Reporte_juego.xlsx
+++ b/Data/Reporte_juego.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y89"/>
+  <dimension ref="A1:Y116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6462,6 +6462,1815 @@
         <v>10</v>
       </c>
     </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2024-11-27 19:21:37</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr"/>
+      <c r="C90" t="n">
+        <v>1</v>
+      </c>
+      <c r="D90" t="n">
+        <v>1</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0</v>
+      </c>
+      <c r="F90" t="n">
+        <v>0</v>
+      </c>
+      <c r="G90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I90" t="inlineStr"/>
+      <c r="J90" t="inlineStr"/>
+      <c r="K90" t="inlineStr"/>
+      <c r="L90" t="inlineStr"/>
+      <c r="M90" t="inlineStr"/>
+      <c r="N90" t="n">
+        <v>10</v>
+      </c>
+      <c r="O90" t="n">
+        <v>7</v>
+      </c>
+      <c r="P90" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q90" t="inlineStr"/>
+      <c r="R90" t="n">
+        <v>6</v>
+      </c>
+      <c r="S90" t="inlineStr"/>
+      <c r="T90" t="n">
+        <v>10</v>
+      </c>
+      <c r="U90" t="inlineStr">
+        <is>
+          <t>12%</t>
+        </is>
+      </c>
+      <c r="V90" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W90" t="inlineStr"/>
+      <c r="X90" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y90" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2024-11-27 19:23:27</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr"/>
+      <c r="C91" t="n">
+        <v>15</v>
+      </c>
+      <c r="D91" t="n">
+        <v>5</v>
+      </c>
+      <c r="E91" t="n">
+        <v>6</v>
+      </c>
+      <c r="F91" t="n">
+        <v>4</v>
+      </c>
+      <c r="G91" t="n">
+        <v>0</v>
+      </c>
+      <c r="H91" t="n">
+        <v>0</v>
+      </c>
+      <c r="I91" t="inlineStr"/>
+      <c r="J91" t="inlineStr"/>
+      <c r="K91" t="inlineStr"/>
+      <c r="L91" t="inlineStr"/>
+      <c r="M91" t="inlineStr"/>
+      <c r="N91" t="n">
+        <v>10</v>
+      </c>
+      <c r="O91" t="n">
+        <v>7</v>
+      </c>
+      <c r="P91" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q91" t="inlineStr"/>
+      <c r="R91" t="n">
+        <v>3</v>
+      </c>
+      <c r="S91" t="inlineStr"/>
+      <c r="T91" t="n">
+        <v>10</v>
+      </c>
+      <c r="U91" t="inlineStr">
+        <is>
+          <t>48%</t>
+        </is>
+      </c>
+      <c r="V91" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W91" t="inlineStr"/>
+      <c r="X91" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y91" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2024-11-27 19:23:42</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr"/>
+      <c r="C92" t="n">
+        <v>0</v>
+      </c>
+      <c r="D92" t="n">
+        <v>0</v>
+      </c>
+      <c r="E92" t="n">
+        <v>0</v>
+      </c>
+      <c r="F92" t="n">
+        <v>0</v>
+      </c>
+      <c r="G92" t="n">
+        <v>0</v>
+      </c>
+      <c r="H92" t="n">
+        <v>0</v>
+      </c>
+      <c r="I92" t="inlineStr"/>
+      <c r="J92" t="inlineStr"/>
+      <c r="K92" t="inlineStr"/>
+      <c r="L92" t="inlineStr"/>
+      <c r="M92" t="inlineStr"/>
+      <c r="N92" t="n">
+        <v>10</v>
+      </c>
+      <c r="O92" t="n">
+        <v>7</v>
+      </c>
+      <c r="P92" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q92" t="inlineStr"/>
+      <c r="R92" t="n">
+        <v>5</v>
+      </c>
+      <c r="S92" t="inlineStr"/>
+      <c r="T92" t="n">
+        <v>20</v>
+      </c>
+      <c r="U92" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V92" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W92" t="inlineStr"/>
+      <c r="X92" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y92" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2024-11-27 19:23:50</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr"/>
+      <c r="C93" t="n">
+        <v>0</v>
+      </c>
+      <c r="D93" t="n">
+        <v>0</v>
+      </c>
+      <c r="E93" t="n">
+        <v>0</v>
+      </c>
+      <c r="F93" t="n">
+        <v>0</v>
+      </c>
+      <c r="G93" t="n">
+        <v>0</v>
+      </c>
+      <c r="H93" t="n">
+        <v>0</v>
+      </c>
+      <c r="I93" t="inlineStr"/>
+      <c r="J93" t="inlineStr"/>
+      <c r="K93" t="inlineStr"/>
+      <c r="L93" t="inlineStr"/>
+      <c r="M93" t="inlineStr"/>
+      <c r="N93" t="n">
+        <v>10</v>
+      </c>
+      <c r="O93" t="n">
+        <v>7</v>
+      </c>
+      <c r="P93" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q93" t="inlineStr"/>
+      <c r="R93" t="n">
+        <v>7</v>
+      </c>
+      <c r="S93" t="inlineStr"/>
+      <c r="T93" t="n">
+        <v>20</v>
+      </c>
+      <c r="U93" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V93" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W93" t="inlineStr"/>
+      <c r="X93" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y93" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2024-11-27 19:28:13</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr"/>
+      <c r="C94" t="n">
+        <v>13</v>
+      </c>
+      <c r="D94" t="n">
+        <v>13</v>
+      </c>
+      <c r="E94" t="n">
+        <v>0</v>
+      </c>
+      <c r="F94" t="n">
+        <v>0</v>
+      </c>
+      <c r="G94" t="n">
+        <v>0</v>
+      </c>
+      <c r="H94" t="n">
+        <v>0</v>
+      </c>
+      <c r="I94" t="inlineStr"/>
+      <c r="J94" t="inlineStr"/>
+      <c r="K94" t="inlineStr"/>
+      <c r="L94" t="inlineStr"/>
+      <c r="M94" t="inlineStr"/>
+      <c r="N94" t="n">
+        <v>10</v>
+      </c>
+      <c r="O94" t="n">
+        <v>7</v>
+      </c>
+      <c r="P94" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q94" t="inlineStr"/>
+      <c r="R94" t="n">
+        <v>7</v>
+      </c>
+      <c r="S94" t="inlineStr"/>
+      <c r="T94" t="n">
+        <v>10</v>
+      </c>
+      <c r="U94" t="inlineStr">
+        <is>
+          <t>30%</t>
+        </is>
+      </c>
+      <c r="V94" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W94" t="inlineStr"/>
+      <c r="X94" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y94" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2024-11-28 06:37:11</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr"/>
+      <c r="C95" t="n">
+        <v>0</v>
+      </c>
+      <c r="D95" t="n">
+        <v>0</v>
+      </c>
+      <c r="E95" t="n">
+        <v>0</v>
+      </c>
+      <c r="F95" t="n">
+        <v>0</v>
+      </c>
+      <c r="G95" t="n">
+        <v>0</v>
+      </c>
+      <c r="H95" t="n">
+        <v>0</v>
+      </c>
+      <c r="I95" t="inlineStr"/>
+      <c r="J95" t="inlineStr"/>
+      <c r="K95" t="inlineStr"/>
+      <c r="L95" t="inlineStr"/>
+      <c r="M95" t="inlineStr"/>
+      <c r="N95" t="n">
+        <v>10</v>
+      </c>
+      <c r="O95" t="n">
+        <v>7</v>
+      </c>
+      <c r="P95" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q95" t="inlineStr"/>
+      <c r="R95" t="n">
+        <v>1</v>
+      </c>
+      <c r="S95" t="inlineStr"/>
+      <c r="T95" t="n">
+        <v>30</v>
+      </c>
+      <c r="U95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V95" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W95" t="inlineStr"/>
+      <c r="X95" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y95" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2024-11-28 06:40:12</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr"/>
+      <c r="C96" t="n">
+        <v>6</v>
+      </c>
+      <c r="D96" t="n">
+        <v>0</v>
+      </c>
+      <c r="E96" t="n">
+        <v>2</v>
+      </c>
+      <c r="F96" t="n">
+        <v>4</v>
+      </c>
+      <c r="G96" t="n">
+        <v>0</v>
+      </c>
+      <c r="H96" t="n">
+        <v>0</v>
+      </c>
+      <c r="I96" t="inlineStr"/>
+      <c r="J96" t="inlineStr"/>
+      <c r="K96" t="inlineStr"/>
+      <c r="L96" t="inlineStr"/>
+      <c r="M96" t="inlineStr"/>
+      <c r="N96" t="n">
+        <v>10</v>
+      </c>
+      <c r="O96" t="n">
+        <v>7</v>
+      </c>
+      <c r="P96" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q96" t="inlineStr"/>
+      <c r="R96" t="n">
+        <v>1</v>
+      </c>
+      <c r="S96" t="inlineStr"/>
+      <c r="T96" t="n">
+        <v>10</v>
+      </c>
+      <c r="U96" t="inlineStr">
+        <is>
+          <t>12%</t>
+        </is>
+      </c>
+      <c r="V96" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W96" t="inlineStr"/>
+      <c r="X96" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y96" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2024-11-28 06:42:18</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr"/>
+      <c r="C97" t="n">
+        <v>5</v>
+      </c>
+      <c r="D97" t="n">
+        <v>0</v>
+      </c>
+      <c r="E97" t="n">
+        <v>3</v>
+      </c>
+      <c r="F97" t="n">
+        <v>2</v>
+      </c>
+      <c r="G97" t="n">
+        <v>0</v>
+      </c>
+      <c r="H97" t="n">
+        <v>0</v>
+      </c>
+      <c r="I97" t="inlineStr"/>
+      <c r="J97" t="inlineStr"/>
+      <c r="K97" t="inlineStr"/>
+      <c r="L97" t="inlineStr"/>
+      <c r="M97" t="inlineStr"/>
+      <c r="N97" t="n">
+        <v>10</v>
+      </c>
+      <c r="O97" t="n">
+        <v>7</v>
+      </c>
+      <c r="P97" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q97" t="inlineStr"/>
+      <c r="R97" t="n">
+        <v>1</v>
+      </c>
+      <c r="S97" t="inlineStr"/>
+      <c r="T97" t="n">
+        <v>40</v>
+      </c>
+      <c r="U97" t="inlineStr">
+        <is>
+          <t>17%</t>
+        </is>
+      </c>
+      <c r="V97" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W97" t="inlineStr"/>
+      <c r="X97" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y97" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2024-11-28 06:45:08</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr"/>
+      <c r="C98" t="n">
+        <v>0</v>
+      </c>
+      <c r="D98" t="n">
+        <v>0</v>
+      </c>
+      <c r="E98" t="n">
+        <v>0</v>
+      </c>
+      <c r="F98" t="n">
+        <v>0</v>
+      </c>
+      <c r="G98" t="n">
+        <v>0</v>
+      </c>
+      <c r="H98" t="n">
+        <v>0</v>
+      </c>
+      <c r="I98" t="inlineStr"/>
+      <c r="J98" t="inlineStr"/>
+      <c r="K98" t="inlineStr"/>
+      <c r="L98" t="inlineStr"/>
+      <c r="M98" t="inlineStr"/>
+      <c r="N98" t="n">
+        <v>10</v>
+      </c>
+      <c r="O98" t="n">
+        <v>7</v>
+      </c>
+      <c r="P98" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q98" t="inlineStr"/>
+      <c r="R98" t="n">
+        <v>5</v>
+      </c>
+      <c r="S98" t="inlineStr"/>
+      <c r="T98" t="n">
+        <v>40</v>
+      </c>
+      <c r="U98" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V98" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W98" t="inlineStr"/>
+      <c r="X98" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y98" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2024-11-28 06:46:30</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr"/>
+      <c r="C99" t="n">
+        <v>6</v>
+      </c>
+      <c r="D99" t="n">
+        <v>2</v>
+      </c>
+      <c r="E99" t="n">
+        <v>3</v>
+      </c>
+      <c r="F99" t="n">
+        <v>1</v>
+      </c>
+      <c r="G99" t="n">
+        <v>0</v>
+      </c>
+      <c r="H99" t="n">
+        <v>0</v>
+      </c>
+      <c r="I99" t="inlineStr"/>
+      <c r="J99" t="inlineStr"/>
+      <c r="K99" t="inlineStr"/>
+      <c r="L99" t="inlineStr"/>
+      <c r="M99" t="inlineStr"/>
+      <c r="N99" t="n">
+        <v>10</v>
+      </c>
+      <c r="O99" t="n">
+        <v>7</v>
+      </c>
+      <c r="P99" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q99" t="inlineStr"/>
+      <c r="R99" t="n">
+        <v>5</v>
+      </c>
+      <c r="S99" t="inlineStr"/>
+      <c r="T99" t="n">
+        <v>40</v>
+      </c>
+      <c r="U99" t="inlineStr">
+        <is>
+          <t>67%</t>
+        </is>
+      </c>
+      <c r="V99" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W99" t="inlineStr"/>
+      <c r="X99" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y99" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2024-12-01 18:30:39</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr"/>
+      <c r="C100" t="n">
+        <v>2</v>
+      </c>
+      <c r="D100" t="n">
+        <v>0</v>
+      </c>
+      <c r="E100" t="n">
+        <v>1</v>
+      </c>
+      <c r="F100" t="n">
+        <v>1</v>
+      </c>
+      <c r="G100" t="n">
+        <v>0</v>
+      </c>
+      <c r="H100" t="n">
+        <v>0</v>
+      </c>
+      <c r="I100" t="inlineStr"/>
+      <c r="J100" t="inlineStr"/>
+      <c r="K100" t="inlineStr"/>
+      <c r="L100" t="inlineStr"/>
+      <c r="M100" t="inlineStr"/>
+      <c r="N100" t="n">
+        <v>10</v>
+      </c>
+      <c r="O100" t="n">
+        <v>7</v>
+      </c>
+      <c r="P100" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q100" t="inlineStr"/>
+      <c r="R100" t="n">
+        <v>3</v>
+      </c>
+      <c r="S100" t="inlineStr"/>
+      <c r="T100" t="n">
+        <v>50</v>
+      </c>
+      <c r="U100" t="inlineStr">
+        <is>
+          <t>29%</t>
+        </is>
+      </c>
+      <c r="V100" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W100" t="inlineStr"/>
+      <c r="X100" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y100" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2024-12-01 18:35:02</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr"/>
+      <c r="C101" t="n">
+        <v>3</v>
+      </c>
+      <c r="D101" t="n">
+        <v>0</v>
+      </c>
+      <c r="E101" t="n">
+        <v>1</v>
+      </c>
+      <c r="F101" t="n">
+        <v>2</v>
+      </c>
+      <c r="G101" t="n">
+        <v>0</v>
+      </c>
+      <c r="H101" t="n">
+        <v>0</v>
+      </c>
+      <c r="I101" t="inlineStr"/>
+      <c r="J101" t="inlineStr"/>
+      <c r="K101" t="inlineStr"/>
+      <c r="L101" t="inlineStr"/>
+      <c r="M101" t="inlineStr"/>
+      <c r="N101" t="n">
+        <v>10</v>
+      </c>
+      <c r="O101" t="n">
+        <v>7</v>
+      </c>
+      <c r="P101" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q101" t="inlineStr"/>
+      <c r="R101" t="n">
+        <v>3</v>
+      </c>
+      <c r="S101" t="inlineStr"/>
+      <c r="T101" t="n">
+        <v>50</v>
+      </c>
+      <c r="U101" t="inlineStr">
+        <is>
+          <t>27%</t>
+        </is>
+      </c>
+      <c r="V101" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W101" t="inlineStr"/>
+      <c r="X101" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y101" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>2024-12-07 21:09:39</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr"/>
+      <c r="C102" t="n">
+        <v>9</v>
+      </c>
+      <c r="D102" t="n">
+        <v>2</v>
+      </c>
+      <c r="E102" t="n">
+        <v>4</v>
+      </c>
+      <c r="F102" t="n">
+        <v>3</v>
+      </c>
+      <c r="G102" t="n">
+        <v>0</v>
+      </c>
+      <c r="H102" t="n">
+        <v>0</v>
+      </c>
+      <c r="I102" t="inlineStr"/>
+      <c r="J102" t="inlineStr"/>
+      <c r="K102" t="inlineStr"/>
+      <c r="L102" t="inlineStr"/>
+      <c r="M102" t="inlineStr"/>
+      <c r="N102" t="n">
+        <v>10</v>
+      </c>
+      <c r="O102" t="n">
+        <v>7</v>
+      </c>
+      <c r="P102" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q102" t="inlineStr"/>
+      <c r="R102" t="n">
+        <v>5</v>
+      </c>
+      <c r="S102" t="inlineStr"/>
+      <c r="T102" t="n">
+        <v>20</v>
+      </c>
+      <c r="U102" t="inlineStr">
+        <is>
+          <t>50%</t>
+        </is>
+      </c>
+      <c r="V102" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W102" t="inlineStr"/>
+      <c r="X102" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y102" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>2024-12-08 23:57:11</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr"/>
+      <c r="C103" t="n">
+        <v>3</v>
+      </c>
+      <c r="D103" t="n">
+        <v>0</v>
+      </c>
+      <c r="E103" t="n">
+        <v>3</v>
+      </c>
+      <c r="F103" t="n">
+        <v>0</v>
+      </c>
+      <c r="G103" t="n">
+        <v>0</v>
+      </c>
+      <c r="H103" t="n">
+        <v>0</v>
+      </c>
+      <c r="I103" t="inlineStr"/>
+      <c r="J103" t="inlineStr"/>
+      <c r="K103" t="inlineStr"/>
+      <c r="L103" t="inlineStr"/>
+      <c r="M103" t="inlineStr"/>
+      <c r="N103" t="n">
+        <v>10</v>
+      </c>
+      <c r="O103" t="n">
+        <v>7</v>
+      </c>
+      <c r="P103" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q103" t="inlineStr"/>
+      <c r="R103" t="n">
+        <v>5</v>
+      </c>
+      <c r="S103" t="inlineStr"/>
+      <c r="T103" t="n">
+        <v>50</v>
+      </c>
+      <c r="U103" t="inlineStr">
+        <is>
+          <t>50%</t>
+        </is>
+      </c>
+      <c r="V103" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W103" t="inlineStr"/>
+      <c r="X103" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y103" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>2024-12-14 22:18:01</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr"/>
+      <c r="C104" t="n">
+        <v>0</v>
+      </c>
+      <c r="D104" t="n">
+        <v>0</v>
+      </c>
+      <c r="E104" t="n">
+        <v>0</v>
+      </c>
+      <c r="F104" t="n">
+        <v>0</v>
+      </c>
+      <c r="G104" t="n">
+        <v>0</v>
+      </c>
+      <c r="H104" t="n">
+        <v>0</v>
+      </c>
+      <c r="I104" t="inlineStr"/>
+      <c r="J104" t="inlineStr"/>
+      <c r="K104" t="inlineStr"/>
+      <c r="L104" t="inlineStr"/>
+      <c r="M104" t="inlineStr"/>
+      <c r="N104" t="n">
+        <v>10</v>
+      </c>
+      <c r="O104" t="n">
+        <v>7</v>
+      </c>
+      <c r="P104" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q104" t="inlineStr"/>
+      <c r="R104" t="n">
+        <v>5</v>
+      </c>
+      <c r="S104" t="inlineStr"/>
+      <c r="T104" t="n">
+        <v>10</v>
+      </c>
+      <c r="U104" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V104" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W104" t="inlineStr"/>
+      <c r="X104" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y104" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>2024-12-15 00:29:09</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr"/>
+      <c r="C105" t="n">
+        <v>20</v>
+      </c>
+      <c r="D105" t="n">
+        <v>4</v>
+      </c>
+      <c r="E105" t="n">
+        <v>10</v>
+      </c>
+      <c r="F105" t="n">
+        <v>6</v>
+      </c>
+      <c r="G105" t="n">
+        <v>0</v>
+      </c>
+      <c r="H105" t="n">
+        <v>0</v>
+      </c>
+      <c r="I105" t="inlineStr"/>
+      <c r="J105" t="inlineStr"/>
+      <c r="K105" t="inlineStr"/>
+      <c r="L105" t="inlineStr"/>
+      <c r="M105" t="inlineStr"/>
+      <c r="N105" t="n">
+        <v>10</v>
+      </c>
+      <c r="O105" t="n">
+        <v>7</v>
+      </c>
+      <c r="P105" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q105" t="inlineStr"/>
+      <c r="R105" t="n">
+        <v>5</v>
+      </c>
+      <c r="S105" t="inlineStr"/>
+      <c r="T105" t="n">
+        <v>20</v>
+      </c>
+      <c r="U105" t="inlineStr">
+        <is>
+          <t>67%</t>
+        </is>
+      </c>
+      <c r="V105" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W105" t="inlineStr"/>
+      <c r="X105" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y105" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>2024-12-15 00:37:30</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr"/>
+      <c r="C106" t="n">
+        <v>4</v>
+      </c>
+      <c r="D106" t="n">
+        <v>1</v>
+      </c>
+      <c r="E106" t="n">
+        <v>2</v>
+      </c>
+      <c r="F106" t="n">
+        <v>1</v>
+      </c>
+      <c r="G106" t="n">
+        <v>0</v>
+      </c>
+      <c r="H106" t="n">
+        <v>0</v>
+      </c>
+      <c r="I106" t="inlineStr"/>
+      <c r="J106" t="inlineStr"/>
+      <c r="K106" t="inlineStr"/>
+      <c r="L106" t="inlineStr"/>
+      <c r="M106" t="inlineStr"/>
+      <c r="N106" t="n">
+        <v>10</v>
+      </c>
+      <c r="O106" t="n">
+        <v>7</v>
+      </c>
+      <c r="P106" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q106" t="inlineStr"/>
+      <c r="R106" t="n">
+        <v>5</v>
+      </c>
+      <c r="S106" t="inlineStr"/>
+      <c r="T106" t="n">
+        <v>1</v>
+      </c>
+      <c r="U106" t="inlineStr">
+        <is>
+          <t>18%</t>
+        </is>
+      </c>
+      <c r="V106" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W106" t="inlineStr"/>
+      <c r="X106" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y106" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>2024-12-15 00:45:26</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr"/>
+      <c r="C107" t="n">
+        <v>52</v>
+      </c>
+      <c r="D107" t="n">
+        <v>10</v>
+      </c>
+      <c r="E107" t="n">
+        <v>23</v>
+      </c>
+      <c r="F107" t="n">
+        <v>19</v>
+      </c>
+      <c r="G107" t="n">
+        <v>0</v>
+      </c>
+      <c r="H107" t="n">
+        <v>0</v>
+      </c>
+      <c r="I107" t="inlineStr"/>
+      <c r="J107" t="inlineStr"/>
+      <c r="K107" t="inlineStr"/>
+      <c r="L107" t="inlineStr"/>
+      <c r="M107" t="inlineStr"/>
+      <c r="N107" t="n">
+        <v>10</v>
+      </c>
+      <c r="O107" t="n">
+        <v>7</v>
+      </c>
+      <c r="P107" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q107" t="inlineStr"/>
+      <c r="R107" t="n">
+        <v>1</v>
+      </c>
+      <c r="S107" t="inlineStr"/>
+      <c r="T107" t="n">
+        <v>1</v>
+      </c>
+      <c r="U107" t="inlineStr">
+        <is>
+          <t>12%</t>
+        </is>
+      </c>
+      <c r="V107" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W107" t="inlineStr"/>
+      <c r="X107" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y107" t="n">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>2024-12-15 13:32:15</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr"/>
+      <c r="C108" t="n">
+        <v>0</v>
+      </c>
+      <c r="D108" t="n">
+        <v>0</v>
+      </c>
+      <c r="E108" t="n">
+        <v>0</v>
+      </c>
+      <c r="F108" t="n">
+        <v>0</v>
+      </c>
+      <c r="G108" t="n">
+        <v>0</v>
+      </c>
+      <c r="H108" t="n">
+        <v>0</v>
+      </c>
+      <c r="I108" t="inlineStr"/>
+      <c r="J108" t="inlineStr"/>
+      <c r="K108" t="inlineStr"/>
+      <c r="L108" t="inlineStr"/>
+      <c r="M108" t="inlineStr"/>
+      <c r="N108" t="n">
+        <v>10</v>
+      </c>
+      <c r="O108" t="n">
+        <v>7</v>
+      </c>
+      <c r="P108" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q108" t="inlineStr"/>
+      <c r="R108" t="n">
+        <v>1</v>
+      </c>
+      <c r="S108" t="inlineStr"/>
+      <c r="T108" t="n">
+        <v>1</v>
+      </c>
+      <c r="U108" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V108" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W108" t="inlineStr"/>
+      <c r="X108" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y108" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>2024-12-15 18:24:49</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr"/>
+      <c r="C109" t="n">
+        <v>0</v>
+      </c>
+      <c r="D109" t="n">
+        <v>0</v>
+      </c>
+      <c r="E109" t="n">
+        <v>0</v>
+      </c>
+      <c r="F109" t="n">
+        <v>0</v>
+      </c>
+      <c r="G109" t="n">
+        <v>0</v>
+      </c>
+      <c r="H109" t="n">
+        <v>0</v>
+      </c>
+      <c r="I109" t="inlineStr"/>
+      <c r="J109" t="inlineStr"/>
+      <c r="K109" t="inlineStr"/>
+      <c r="L109" t="inlineStr"/>
+      <c r="M109" t="inlineStr"/>
+      <c r="N109" t="n">
+        <v>10</v>
+      </c>
+      <c r="O109" t="n">
+        <v>7</v>
+      </c>
+      <c r="P109" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q109" t="inlineStr"/>
+      <c r="R109" t="n">
+        <v>5</v>
+      </c>
+      <c r="S109" t="inlineStr"/>
+      <c r="T109" t="n">
+        <v>15</v>
+      </c>
+      <c r="U109" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V109" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W109" t="inlineStr"/>
+      <c r="X109" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y109" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>2024-12-15 18:25:25</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr"/>
+      <c r="C110" t="n">
+        <v>0</v>
+      </c>
+      <c r="D110" t="n">
+        <v>0</v>
+      </c>
+      <c r="E110" t="n">
+        <v>0</v>
+      </c>
+      <c r="F110" t="n">
+        <v>0</v>
+      </c>
+      <c r="G110" t="n">
+        <v>0</v>
+      </c>
+      <c r="H110" t="n">
+        <v>0</v>
+      </c>
+      <c r="I110" t="inlineStr"/>
+      <c r="J110" t="inlineStr"/>
+      <c r="K110" t="inlineStr"/>
+      <c r="L110" t="inlineStr"/>
+      <c r="M110" t="inlineStr"/>
+      <c r="N110" t="n">
+        <v>10</v>
+      </c>
+      <c r="O110" t="n">
+        <v>7</v>
+      </c>
+      <c r="P110" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q110" t="inlineStr"/>
+      <c r="R110" t="n">
+        <v>1</v>
+      </c>
+      <c r="S110" t="inlineStr"/>
+      <c r="T110" t="n">
+        <v>15</v>
+      </c>
+      <c r="U110" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V110" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Crupier.xlsx</t>
+        </is>
+      </c>
+      <c r="W110" t="inlineStr"/>
+      <c r="X110" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y110" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>2024-12-15 20:52:44</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr"/>
+      <c r="C111" t="n">
+        <v>0</v>
+      </c>
+      <c r="D111" t="n">
+        <v>0</v>
+      </c>
+      <c r="E111" t="n">
+        <v>0</v>
+      </c>
+      <c r="F111" t="n">
+        <v>0</v>
+      </c>
+      <c r="G111" t="n">
+        <v>0</v>
+      </c>
+      <c r="H111" t="n">
+        <v>0</v>
+      </c>
+      <c r="I111" t="inlineStr"/>
+      <c r="J111" t="inlineStr"/>
+      <c r="K111" t="inlineStr"/>
+      <c r="L111" t="inlineStr"/>
+      <c r="M111" t="inlineStr"/>
+      <c r="N111" t="n">
+        <v>10</v>
+      </c>
+      <c r="O111" t="n">
+        <v>7</v>
+      </c>
+      <c r="P111" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q111" t="inlineStr"/>
+      <c r="R111" t="n">
+        <v>1</v>
+      </c>
+      <c r="S111" t="inlineStr"/>
+      <c r="T111" t="n">
+        <v>20</v>
+      </c>
+      <c r="U111" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="V111" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W111" t="inlineStr"/>
+      <c r="X111" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y111" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2024-12-15 22:43:59</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr"/>
+      <c r="C112" t="n">
+        <v>3</v>
+      </c>
+      <c r="D112" t="n">
+        <v>3</v>
+      </c>
+      <c r="E112" t="n">
+        <v>0</v>
+      </c>
+      <c r="F112" t="n">
+        <v>0</v>
+      </c>
+      <c r="G112" t="n">
+        <v>0</v>
+      </c>
+      <c r="H112" t="n">
+        <v>0</v>
+      </c>
+      <c r="I112" t="inlineStr"/>
+      <c r="J112" t="inlineStr"/>
+      <c r="K112" t="inlineStr"/>
+      <c r="L112" t="inlineStr"/>
+      <c r="M112" t="inlineStr"/>
+      <c r="N112" t="n">
+        <v>10</v>
+      </c>
+      <c r="O112" t="n">
+        <v>7</v>
+      </c>
+      <c r="P112" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q112" t="inlineStr"/>
+      <c r="R112" t="n">
+        <v>1</v>
+      </c>
+      <c r="S112" t="inlineStr"/>
+      <c r="T112" t="n">
+        <v>50</v>
+      </c>
+      <c r="U112" t="inlineStr">
+        <is>
+          <t>3%</t>
+        </is>
+      </c>
+      <c r="V112" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W112" t="inlineStr"/>
+      <c r="X112" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y112" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2024-12-15 23:06:14</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr"/>
+      <c r="C113" t="n">
+        <v>0</v>
+      </c>
+      <c r="D113" t="n">
+        <v>0</v>
+      </c>
+      <c r="E113" t="n">
+        <v>0</v>
+      </c>
+      <c r="F113" t="n">
+        <v>0</v>
+      </c>
+      <c r="G113" t="n">
+        <v>0</v>
+      </c>
+      <c r="H113" t="n">
+        <v>0</v>
+      </c>
+      <c r="I113" t="inlineStr"/>
+      <c r="J113" t="inlineStr"/>
+      <c r="K113" t="inlineStr"/>
+      <c r="L113" t="inlineStr"/>
+      <c r="M113" t="inlineStr"/>
+      <c r="N113" t="n">
+        <v>10</v>
+      </c>
+      <c r="O113" t="n">
+        <v>7</v>
+      </c>
+      <c r="P113" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q113" t="inlineStr"/>
+      <c r="R113" t="n">
+        <v>1</v>
+      </c>
+      <c r="S113" t="inlineStr"/>
+      <c r="T113" t="n">
+        <v>70</v>
+      </c>
+      <c r="U113" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
+      </c>
+      <c r="V113" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W113" t="inlineStr"/>
+      <c r="X113" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y113" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2024-12-15 23:47:58</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr"/>
+      <c r="C114" t="n">
+        <v>19</v>
+      </c>
+      <c r="D114" t="n">
+        <v>6</v>
+      </c>
+      <c r="E114" t="n">
+        <v>13</v>
+      </c>
+      <c r="F114" t="n">
+        <v>0</v>
+      </c>
+      <c r="G114" t="n">
+        <v>0</v>
+      </c>
+      <c r="H114" t="n">
+        <v>0</v>
+      </c>
+      <c r="I114" t="inlineStr"/>
+      <c r="J114" t="inlineStr"/>
+      <c r="K114" t="inlineStr"/>
+      <c r="L114" t="inlineStr"/>
+      <c r="M114" t="inlineStr"/>
+      <c r="N114" t="n">
+        <v>10</v>
+      </c>
+      <c r="O114" t="n">
+        <v>7</v>
+      </c>
+      <c r="P114" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q114" t="inlineStr"/>
+      <c r="R114" t="n">
+        <v>1</v>
+      </c>
+      <c r="S114" t="inlineStr"/>
+      <c r="T114" t="n">
+        <v>90</v>
+      </c>
+      <c r="U114" t="inlineStr">
+        <is>
+          <t>6%</t>
+        </is>
+      </c>
+      <c r="V114" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W114" t="inlineStr"/>
+      <c r="X114" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y114" t="n">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>2024-12-16 00:46:16</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr"/>
+      <c r="C115" t="n">
+        <v>9</v>
+      </c>
+      <c r="D115" t="n">
+        <v>0</v>
+      </c>
+      <c r="E115" t="n">
+        <v>6</v>
+      </c>
+      <c r="F115" t="n">
+        <v>3</v>
+      </c>
+      <c r="G115" t="n">
+        <v>0</v>
+      </c>
+      <c r="H115" t="n">
+        <v>0</v>
+      </c>
+      <c r="I115" t="inlineStr"/>
+      <c r="J115" t="inlineStr"/>
+      <c r="K115" t="inlineStr"/>
+      <c r="L115" t="inlineStr"/>
+      <c r="M115" t="inlineStr"/>
+      <c r="N115" t="n">
+        <v>10</v>
+      </c>
+      <c r="O115" t="n">
+        <v>7</v>
+      </c>
+      <c r="P115" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q115" t="inlineStr"/>
+      <c r="R115" t="n">
+        <v>1</v>
+      </c>
+      <c r="S115" t="inlineStr"/>
+      <c r="T115" t="n">
+        <v>90</v>
+      </c>
+      <c r="U115" t="inlineStr">
+        <is>
+          <t>82%</t>
+        </is>
+      </c>
+      <c r="V115" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W115" t="inlineStr"/>
+      <c r="X115" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y115" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2024-12-16 01:16:41</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr"/>
+      <c r="C116" t="n">
+        <v>2</v>
+      </c>
+      <c r="D116" t="n">
+        <v>2</v>
+      </c>
+      <c r="E116" t="n">
+        <v>0</v>
+      </c>
+      <c r="F116" t="n">
+        <v>0</v>
+      </c>
+      <c r="G116" t="n">
+        <v>0</v>
+      </c>
+      <c r="H116" t="n">
+        <v>0</v>
+      </c>
+      <c r="I116" t="inlineStr"/>
+      <c r="J116" t="inlineStr"/>
+      <c r="K116" t="inlineStr"/>
+      <c r="L116" t="inlineStr"/>
+      <c r="M116" t="inlineStr"/>
+      <c r="N116" t="n">
+        <v>10</v>
+      </c>
+      <c r="O116" t="n">
+        <v>7</v>
+      </c>
+      <c r="P116" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q116" t="inlineStr"/>
+      <c r="R116" t="n">
+        <v>1</v>
+      </c>
+      <c r="S116" t="inlineStr"/>
+      <c r="T116" t="n">
+        <v>50</v>
+      </c>
+      <c r="U116" t="inlineStr">
+        <is>
+          <t>29%</t>
+        </is>
+      </c>
+      <c r="V116" t="inlineStr">
+        <is>
+          <t>D:\Repositorio\jonatha1992\Predictor_ruleta\Data\Electromecanica.xlsx</t>
+        </is>
+      </c>
+      <c r="W116" t="inlineStr"/>
+      <c r="X116" t="inlineStr">
+        <is>
+          <t>No es Simulación</t>
+        </is>
+      </c>
+      <c r="Y116" t="n">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>